<commit_message>
Updated- Login,Home and register Modules
</commit_message>
<xml_diff>
--- a/src/test/resources/excelTestData/DsAlgoTestData.xlsx
+++ b/src/test/resources/excelTestData/DsAlgoTestData.xlsx
@@ -1,13 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Desktop\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53374884-6F93-433A-9191-B89E7F931C4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="LoginData" sheetId="1" r:id="rId1"/>
+    <sheet name="RegisterData" sheetId="2" r:id="rId2"/>
+    <sheet name="Pages" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -18,12 +26,79 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>qa123123</t>
+  </si>
+  <si>
+    <t>testing@8</t>
+  </si>
+  <si>
+    <t>EditorCode</t>
+  </si>
+  <si>
+    <t>print("Hello, World!")</t>
+  </si>
+  <si>
+    <t>Valid Username</t>
+  </si>
+  <si>
+    <t>Valid Password</t>
+  </si>
+  <si>
+    <t>Valid ConfirmPassword</t>
+  </si>
+  <si>
+    <t>Invalid Username</t>
+  </si>
+  <si>
+    <t>Invalid Password</t>
+  </si>
+  <si>
+    <t>Invalid Confirm Password</t>
+  </si>
+  <si>
+    <t>qa111222</t>
+  </si>
+  <si>
+    <t>testing@123</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> testing@123456</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -46,13 +121,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -330,13 +416,158 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="14.42578125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{48068059-5C3A-405C-9F1E-8FD343F696B6}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D89A5F12-D547-483D-A7F1-F3E683450B23}">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19" style="1" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="22.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="1">
+        <v>123</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E3" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E4" s="1">
+        <v>12345678</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C4B8EA8-C63D-4AA8-9745-DF4AE525FD34}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>